<commit_message>
timesheet fill till 25/03/2022
</commit_message>
<xml_diff>
--- a/rishabh_timesheet.xlsx
+++ b/rishabh_timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55683\OneDrive - ICF\Desktop\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC84C30-6909-477F-9349-B8AE4E6DD1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D1DFD9-5FE4-4EFE-A786-A43C77A020D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{91D1710D-DA54-4467-A82A-013A3D0A24E4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="92">
   <si>
     <t>CODE</t>
   </si>
@@ -384,6 +384,37 @@
   <si>
     <t>Working on Indices Automation Task 
 working on services of indices automation task</t>
+  </si>
+  <si>
+    <t>CRISIL NEW PROJECT CODE</t>
+  </si>
+  <si>
+    <t>163687.0.002.01</t>
+  </si>
+  <si>
+    <t>PTO (015002)</t>
+  </si>
+  <si>
+    <t>Learning SOLR concept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working on SOLR Services Implementation part of CRISIL Indices Automation </t>
+  </si>
+  <si>
+    <t>Working on SOLR Services Implementation part of CRISIL Indices Automation as well as OSGi configuration of API.</t>
+  </si>
+  <si>
+    <t>Working on SOLR Services CRUD operation
+written method for adding data into the SOLR
+written method for getting data into the SOLR
+written method for deleting data using uniqueKey to the SOLR.</t>
+  </si>
+  <si>
+    <t>Working on SOLR Services CRUD operation
+written method for adding data into the SOLR
+written method for getting data into the SOLR
+written method for deleting data using uniqueKey to the SOLR.
+Adding some required configuration of SOLR.</t>
   </si>
 </sst>
 </file>
@@ -507,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,6 +624,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -602,17 +636,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -934,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8568C51-A3B1-4ED9-851C-00FAAEFAC243}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,6 +1036,14 @@
         <v>61</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1012,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C3AD78-21C2-40ED-A814-165D4FC13558}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,7 +1098,7 @@
       <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="30">
         <v>44564</v>
       </c>
       <c r="E2" s="21" t="s">
@@ -1076,7 +1118,7 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="21" t="s">
         <v>6</v>
       </c>
@@ -1094,7 +1136,7 @@
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="30">
         <v>44565</v>
       </c>
       <c r="E4" s="21" t="s">
@@ -1114,7 +1156,7 @@
       <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="21" t="s">
         <v>20</v>
       </c>
@@ -1132,7 +1174,7 @@
       <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="30">
         <v>44566</v>
       </c>
       <c r="E6" s="22" t="s">
@@ -1152,7 +1194,7 @@
       <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="31"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="4"/>
       <c r="F7" s="19"/>
     </row>
@@ -1166,7 +1208,7 @@
       <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="30">
         <v>44567</v>
       </c>
       <c r="E8" s="24"/>
@@ -1182,7 +1224,7 @@
       <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
     </row>
@@ -1196,7 +1238,7 @@
       <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="30">
         <v>44568</v>
       </c>
       <c r="E10" s="24"/>
@@ -1212,7 +1254,7 @@
       <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
     </row>
@@ -1242,7 +1284,7 @@
       <c r="C13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="30">
         <v>44572</v>
       </c>
       <c r="E13" s="24"/>
@@ -1258,7 +1300,7 @@
       <c r="C14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
     </row>
@@ -1272,7 +1314,7 @@
       <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="30">
         <v>44573</v>
       </c>
       <c r="E15" s="24"/>
@@ -1288,7 +1330,7 @@
       <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
     </row>
@@ -1318,7 +1360,7 @@
       <c r="C18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="30">
         <v>44578</v>
       </c>
       <c r="E18" s="24"/>
@@ -1334,7 +1376,7 @@
       <c r="C19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
     </row>
@@ -1364,7 +1406,7 @@
       <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="30">
         <v>44580</v>
       </c>
     </row>
@@ -1378,7 +1420,7 @@
       <c r="C22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
@@ -1390,7 +1432,7 @@
       <c r="C23" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="30">
         <v>44581</v>
       </c>
     </row>
@@ -1404,7 +1446,7 @@
       <c r="C24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="30"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -1444,7 +1486,7 @@
       <c r="C27" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="30">
         <v>44586</v>
       </c>
     </row>
@@ -1458,7 +1500,7 @@
       <c r="C28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="30"/>
     </row>
     <row r="29" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
@@ -1470,7 +1512,7 @@
       <c r="C29" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="30">
         <v>44588</v>
       </c>
     </row>
@@ -1484,7 +1526,7 @@
       <c r="C30" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
@@ -1496,7 +1538,7 @@
       <c r="C31" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="30">
         <v>44589</v>
       </c>
     </row>
@@ -1510,7 +1552,7 @@
       <c r="C32" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
@@ -1522,7 +1564,7 @@
       <c r="C33" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="29">
+      <c r="D33" s="30">
         <v>44592</v>
       </c>
     </row>
@@ -1536,16 +1578,10 @@
       <c r="C34" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="29"/>
+      <c r="D34" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D13:D14"/>
@@ -1554,6 +1590,12 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1565,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD25E0C-56B4-49C9-81FC-B33B23DE8FF6}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1599,7 +1641,7 @@
       <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="36">
         <v>44593</v>
       </c>
     </row>
@@ -1613,7 +1655,7 @@
       <c r="C3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1625,7 +1667,7 @@
       <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="36">
         <v>44594</v>
       </c>
     </row>
@@ -1639,7 +1681,7 @@
       <c r="C5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1651,7 +1693,7 @@
       <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="36">
         <v>44595</v>
       </c>
     </row>
@@ -1665,7 +1707,7 @@
       <c r="C7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="32"/>
+      <c r="D7" s="36"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1677,7 +1719,7 @@
       <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="36">
         <v>44596</v>
       </c>
     </row>
@@ -1691,7 +1733,7 @@
       <c r="C9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1703,7 +1745,7 @@
       <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="36">
         <v>44599</v>
       </c>
     </row>
@@ -1717,7 +1759,7 @@
       <c r="C11" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1729,7 +1771,7 @@
       <c r="C12" s="4">
         <v>4</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="36">
         <v>44600</v>
       </c>
     </row>
@@ -1743,7 +1785,7 @@
       <c r="C13" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="36"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1755,7 +1797,7 @@
       <c r="C14" s="4">
         <v>4</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="36">
         <v>44601</v>
       </c>
     </row>
@@ -1769,7 +1811,7 @@
       <c r="C15" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="36"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -1781,7 +1823,7 @@
       <c r="C16" s="4">
         <v>4</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="36">
         <v>44602</v>
       </c>
     </row>
@@ -1795,7 +1837,7 @@
       <c r="C17" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="36"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -1807,7 +1849,7 @@
       <c r="C18" s="4">
         <v>4</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="36">
         <v>44603</v>
       </c>
     </row>
@@ -1821,7 +1863,7 @@
       <c r="C19" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="32"/>
+      <c r="D19" s="36"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -1833,7 +1875,7 @@
       <c r="C20" s="4">
         <v>4</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="36">
         <v>44606</v>
       </c>
     </row>
@@ -1847,7 +1889,7 @@
       <c r="C21" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="32"/>
+      <c r="D21" s="36"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -1859,7 +1901,7 @@
       <c r="C22" s="4">
         <v>4</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="36">
         <v>44607</v>
       </c>
     </row>
@@ -1873,7 +1915,7 @@
       <c r="C23" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="36"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -1883,7 +1925,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="34"/>
-      <c r="D24" s="32">
+      <c r="D24" s="36">
         <v>44608</v>
       </c>
     </row>
@@ -1895,7 +1937,7 @@
         <v>57</v>
       </c>
       <c r="C25" s="35"/>
-      <c r="D25" s="32"/>
+      <c r="D25" s="36"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -1907,7 +1949,7 @@
       <c r="C26" s="4">
         <v>4</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="36">
         <v>44609</v>
       </c>
     </row>
@@ -1921,7 +1963,7 @@
       <c r="C27" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="36"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -1933,7 +1975,7 @@
       <c r="C28" s="4">
         <v>4</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="36">
         <v>44610</v>
       </c>
     </row>
@@ -1947,7 +1989,7 @@
       <c r="C29" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="32"/>
+      <c r="D29" s="36"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
@@ -1959,7 +2001,7 @@
       <c r="C30" s="4">
         <v>4</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="36">
         <v>44613</v>
       </c>
     </row>
@@ -1973,7 +2015,7 @@
       <c r="C31" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="32"/>
+      <c r="D31" s="36"/>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
@@ -1997,7 +2039,7 @@
       <c r="C33" s="4">
         <v>0</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="36">
         <v>44614</v>
       </c>
     </row>
@@ -2009,7 +2051,7 @@
         <v>63</v>
       </c>
       <c r="C34" s="17"/>
-      <c r="D34" s="32"/>
+      <c r="D34" s="36"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
@@ -2021,7 +2063,7 @@
       <c r="C35" s="4">
         <v>0</v>
       </c>
-      <c r="D35" s="32">
+      <c r="D35" s="36">
         <v>44615</v>
       </c>
     </row>
@@ -2033,7 +2075,7 @@
         <v>64</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="32"/>
+      <c r="D36" s="36"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
@@ -2045,7 +2087,7 @@
       <c r="C37" s="4">
         <v>0</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="36">
         <v>44616</v>
       </c>
     </row>
@@ -2057,7 +2099,7 @@
         <v>66</v>
       </c>
       <c r="C38" s="17"/>
-      <c r="D38" s="32"/>
+      <c r="D38" s="36"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
@@ -2069,7 +2111,7 @@
       <c r="C39" s="4">
         <v>0</v>
       </c>
-      <c r="D39" s="32">
+      <c r="D39" s="36">
         <v>44617</v>
       </c>
     </row>
@@ -2081,7 +2123,7 @@
         <v>67</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="32"/>
+      <c r="D40" s="36"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
@@ -2093,7 +2135,7 @@
       <c r="C41" s="4">
         <v>0</v>
       </c>
-      <c r="D41" s="32">
+      <c r="D41" s="36">
         <v>44618</v>
       </c>
     </row>
@@ -2105,7 +2147,7 @@
         <v>67</v>
       </c>
       <c r="C42" s="17"/>
-      <c r="D42" s="32"/>
+      <c r="D42" s="36"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
@@ -2117,7 +2159,7 @@
       <c r="C43" s="4">
         <v>0</v>
       </c>
-      <c r="D43" s="32">
+      <c r="D43" s="36">
         <v>44619</v>
       </c>
     </row>
@@ -2129,7 +2171,7 @@
         <v>68</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="32"/>
+      <c r="D44" s="36"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
@@ -2141,7 +2183,7 @@
       <c r="C45" s="4">
         <v>0</v>
       </c>
-      <c r="D45" s="32">
+      <c r="D45" s="36">
         <v>44620</v>
       </c>
     </row>
@@ -2153,22 +2195,10 @@
         <v>69</v>
       </c>
       <c r="C46" s="17"/>
-      <c r="D46" s="32"/>
+      <c r="D46" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
     <mergeCell ref="D39:D40"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D43:D44"/>
@@ -2181,6 +2211,18 @@
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2189,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38664062-6459-4C38-9B3B-3A164047A9A0}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2219,11 +2261,11 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36">
-        <v>8</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="32">
+      <c r="B2" s="37">
+        <v>8</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="36">
         <v>44621</v>
       </c>
     </row>
@@ -2235,7 +2277,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="35"/>
-      <c r="D3" s="32"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -2247,7 +2289,7 @@
       <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="36">
         <v>44622</v>
       </c>
     </row>
@@ -2259,7 +2301,7 @@
         <v>70</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="32"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -2271,7 +2313,7 @@
       <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="36">
         <v>44623</v>
       </c>
     </row>
@@ -2283,7 +2325,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="32"/>
+      <c r="D7" s="36"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -2295,7 +2337,7 @@
       <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="36">
         <v>44624</v>
       </c>
     </row>
@@ -2307,7 +2349,7 @@
         <v>72</v>
       </c>
       <c r="C9" s="17"/>
-      <c r="D9" s="32"/>
+      <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -2319,7 +2361,7 @@
       <c r="C10" s="4">
         <v>0</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="36">
         <v>44627</v>
       </c>
     </row>
@@ -2331,7 +2373,7 @@
         <v>76</v>
       </c>
       <c r="C11" s="17"/>
-      <c r="D11" s="32"/>
+      <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -2343,7 +2385,7 @@
       <c r="C12" s="4">
         <v>0</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="36">
         <v>44628</v>
       </c>
     </row>
@@ -2355,7 +2397,7 @@
         <v>79</v>
       </c>
       <c r="C13" s="17"/>
-      <c r="D13" s="32"/>
+      <c r="D13" s="36"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -2367,7 +2409,7 @@
       <c r="C14" s="4">
         <v>0</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="36">
         <v>44629</v>
       </c>
     </row>
@@ -2379,7 +2421,7 @@
         <v>78</v>
       </c>
       <c r="C15" s="17"/>
-      <c r="D15" s="32"/>
+      <c r="D15" s="36"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -2391,7 +2433,7 @@
       <c r="C16" s="4">
         <v>0</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="36">
         <v>44630</v>
       </c>
     </row>
@@ -2403,7 +2445,7 @@
         <v>77</v>
       </c>
       <c r="C17" s="17"/>
-      <c r="D17" s="32"/>
+      <c r="D17" s="36"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -2415,7 +2457,7 @@
       <c r="C18" s="4">
         <v>4</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="36">
         <v>44631</v>
       </c>
     </row>
@@ -2429,7 +2471,7 @@
       <c r="C19" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="32"/>
+      <c r="D19" s="36"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -2441,7 +2483,7 @@
       <c r="C20" s="4">
         <v>0</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="36">
         <v>44634</v>
       </c>
     </row>
@@ -2453,7 +2495,7 @@
         <v>75</v>
       </c>
       <c r="C21" s="17"/>
-      <c r="D21" s="32"/>
+      <c r="D21" s="36"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -2465,7 +2507,7 @@
       <c r="C22" s="4">
         <v>0</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="36">
         <v>44635</v>
       </c>
     </row>
@@ -2477,7 +2519,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="17"/>
-      <c r="D23" s="32"/>
+      <c r="D23" s="36"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -2489,7 +2531,7 @@
       <c r="C24" s="4">
         <v>0</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="36">
         <v>44636</v>
       </c>
     </row>
@@ -2501,7 +2543,7 @@
         <v>82</v>
       </c>
       <c r="C25" s="17"/>
-      <c r="D25" s="32"/>
+      <c r="D25" s="36"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -2513,7 +2555,7 @@
       <c r="C26" s="4">
         <v>0</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="36">
         <v>44637</v>
       </c>
     </row>
@@ -2525,7 +2567,7 @@
         <v>83</v>
       </c>
       <c r="C27" s="17"/>
-      <c r="D27" s="32"/>
+      <c r="D27" s="36"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -2535,7 +2577,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="34"/>
-      <c r="D28" s="32">
+      <c r="D28" s="36">
         <v>44638</v>
       </c>
     </row>
@@ -2547,37 +2589,165 @@
         <v>81</v>
       </c>
       <c r="C29" s="34"/>
-      <c r="D29" s="32"/>
+      <c r="D29" s="36"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="15">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C30" s="4">
-        <v>0</v>
-      </c>
-      <c r="D30" s="32">
+        <v>6</v>
+      </c>
+      <c r="D30" s="36">
         <v>44641</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="32"/>
+      <c r="B31" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="36"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="15">
+        <v>2</v>
+      </c>
+      <c r="C32" s="4">
+        <v>6</v>
+      </c>
+      <c r="D32" s="36">
+        <v>44642</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="36"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="15">
+        <v>2</v>
+      </c>
+      <c r="C34" s="4">
+        <v>6</v>
+      </c>
+      <c r="D34" s="36">
+        <v>44643</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="36"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="15">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4">
+        <v>6</v>
+      </c>
+      <c r="D36" s="36">
+        <v>44644</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="36"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="33">
+        <v>8</v>
+      </c>
+      <c r="C38" s="34"/>
+      <c r="D38" s="36">
+        <v>44645</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="34"/>
+      <c r="D39" s="36"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="33">
+        <v>8</v>
+      </c>
+      <c r="C40" s="34"/>
+      <c r="D40" s="36">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="34"/>
+      <c r="D41" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
+  <mergeCells count="28">
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D12:D13"/>
@@ -2585,13 +2755,20 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B39:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2599,6 +2776,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010071FEBA6E59F1114FA1DBADB5A19192F5" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="68d738ba6abfae8d013aeb1fb6af46ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="33e4e33d-ffb4-4a17-9b1b-478bea8d3710" xmlns:ns4="9120eac6-4b18-4abe-a762-bd257214a810" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dae310c37f0a31cfa956236035f6b2a5" ns3:_="" ns4:_="">
     <xsd:import namespace="33e4e33d-ffb4-4a17-9b1b-478bea8d3710"/>
@@ -2807,22 +2999,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD282290-682D-4720-AA66-05DB34A587D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="33e4e33d-ffb4-4a17-9b1b-478bea8d3710"/>
+    <ds:schemaRef ds:uri="9120eac6-4b18-4abe-a762-bd257214a810"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81EA1DDF-0A41-4AEA-8848-5B89771E278B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{248AF9C3-A2BF-4479-B7A8-B2BDE179A582}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2839,29 +3041,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81EA1DDF-0A41-4AEA-8848-5B89771E278B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD282290-682D-4720-AA66-05DB34A587D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="33e4e33d-ffb4-4a17-9b1b-478bea8d3710"/>
-    <ds:schemaRef ds:uri="9120eac6-4b18-4abe-a762-bd257214a810"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
demo html page for downloding excel and pdf from html data
</commit_message>
<xml_diff>
--- a/rishabh_timesheet.xlsx
+++ b/rishabh_timesheet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55683\OneDrive - ICF\Desktop\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D1DFD9-5FE4-4EFE-A786-A43C77A020D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A7EE5E-CF11-4AF8-8964-35C976966327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{91D1710D-DA54-4467-A82A-013A3D0A24E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{91D1710D-DA54-4467-A82A-013A3D0A24E4}"/>
   </bookViews>
   <sheets>
     <sheet name="CODE" sheetId="2" r:id="rId1"/>
     <sheet name="January" sheetId="1" r:id="rId2"/>
     <sheet name="February" sheetId="3" r:id="rId3"/>
     <sheet name="March" sheetId="4" r:id="rId4"/>
+    <sheet name="April" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="100">
   <si>
     <t>CODE</t>
   </si>
@@ -398,23 +399,64 @@
     <t>Learning SOLR concept</t>
   </si>
   <si>
-    <t xml:space="preserve">Working on SOLR Services Implementation part of CRISIL Indices Automation </t>
-  </si>
-  <si>
-    <t>Working on SOLR Services Implementation part of CRISIL Indices Automation as well as OSGi configuration of API.</t>
-  </si>
-  <si>
-    <t>Working on SOLR Services CRUD operation
+    <t>Project: Crisil
+Task: CR
+Task Detail: Working on SOLR Services Implementation part of CRISIL Indices Automation.</t>
+  </si>
+  <si>
+    <t>Project: Crisil
+Task: CR
+Task Detail: Working on SOLR Services Implementation part of CRISIL Indices Automation as well as OSGi configuration of API.</t>
+  </si>
+  <si>
+    <t>Project: Crisil
+Task: CR
+Task Detail: Working on SOLR Services CRUD operation
 written method for adding data into the SOLR
 written method for getting data into the SOLR
 written method for deleting data using uniqueKey to the SOLR.</t>
   </si>
   <si>
-    <t>Working on SOLR Services CRUD operation
+    <t>Project: Crisil
+Task: CR
+Task Detail: Working on SOLR Services CRUD operation
 written method for adding data into the SOLR
 written method for getting data into the SOLR
 written method for deleting data using uniqueKey to the SOLR.
 Adding some required configuration of SOLR.</t>
+  </si>
+  <si>
+    <t>Learning how to use run mode</t>
+  </si>
+  <si>
+    <t>Learn how to set configuration locally for solr</t>
+  </si>
+  <si>
+    <t>Project: Crisil
+Task: CR
+Task Detail: Write Crud operation for solr</t>
+  </si>
+  <si>
+    <t>Project: Crisil
+Task: CR 
+Task Detail: writing services for the indices</t>
+  </si>
+  <si>
+    <t>CRISIL CODE
+163687.0.002.01</t>
+  </si>
+  <si>
+    <t>Project: Crisil
+Task: CR 
+Task Detail: testing services for the indices</t>
+  </si>
+  <si>
+    <t>learn different types of run modes and how to use them.</t>
+  </si>
+  <si>
+    <t>Project: Crisil
+Task: CR 
+Task Detail: working on services part for the indices automation task</t>
   </si>
 </sst>
 </file>
@@ -538,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -627,6 +669,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,6 +681,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -644,9 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1098,7 +1143,7 @@
       <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="31">
         <v>44564</v>
       </c>
       <c r="E2" s="21" t="s">
@@ -1118,7 +1163,7 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="21" t="s">
         <v>6</v>
       </c>
@@ -1136,7 +1181,7 @@
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="31">
         <v>44565</v>
       </c>
       <c r="E4" s="21" t="s">
@@ -1156,7 +1201,7 @@
       <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="21" t="s">
         <v>20</v>
       </c>
@@ -1174,7 +1219,7 @@
       <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="31">
         <v>44566</v>
       </c>
       <c r="E6" s="22" t="s">
@@ -1194,7 +1239,7 @@
       <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="32"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="4"/>
       <c r="F7" s="19"/>
     </row>
@@ -1208,7 +1253,7 @@
       <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="31">
         <v>44567</v>
       </c>
       <c r="E8" s="24"/>
@@ -1224,7 +1269,7 @@
       <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="31"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
     </row>
@@ -1238,7 +1283,7 @@
       <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="31">
         <v>44568</v>
       </c>
       <c r="E10" s="24"/>
@@ -1254,7 +1299,7 @@
       <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
     </row>
@@ -1284,7 +1329,7 @@
       <c r="C13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="31">
         <v>44572</v>
       </c>
       <c r="E13" s="24"/>
@@ -1300,7 +1345,7 @@
       <c r="C14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
     </row>
@@ -1314,7 +1359,7 @@
       <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="31">
         <v>44573</v>
       </c>
       <c r="E15" s="24"/>
@@ -1330,7 +1375,7 @@
       <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="30"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
     </row>
@@ -1360,7 +1405,7 @@
       <c r="C18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="31">
         <v>44578</v>
       </c>
       <c r="E18" s="24"/>
@@ -1376,7 +1421,7 @@
       <c r="C19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
     </row>
@@ -1406,7 +1451,7 @@
       <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="31">
         <v>44580</v>
       </c>
     </row>
@@ -1420,7 +1465,7 @@
       <c r="C22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
@@ -1432,7 +1477,7 @@
       <c r="C23" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="31">
         <v>44581</v>
       </c>
     </row>
@@ -1446,7 +1491,7 @@
       <c r="C24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="30"/>
+      <c r="D24" s="31"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -1486,7 +1531,7 @@
       <c r="C27" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="30">
+      <c r="D27" s="31">
         <v>44586</v>
       </c>
     </row>
@@ -1500,7 +1545,7 @@
       <c r="C28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="30"/>
+      <c r="D28" s="31"/>
     </row>
     <row r="29" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
@@ -1512,7 +1557,7 @@
       <c r="C29" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="30">
+      <c r="D29" s="31">
         <v>44588</v>
       </c>
     </row>
@@ -1526,7 +1571,7 @@
       <c r="C30" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="30"/>
+      <c r="D30" s="31"/>
     </row>
     <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
@@ -1538,7 +1583,7 @@
       <c r="C31" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="30">
+      <c r="D31" s="31">
         <v>44589</v>
       </c>
     </row>
@@ -1552,7 +1597,7 @@
       <c r="C32" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="30"/>
+      <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
@@ -1564,7 +1609,7 @@
       <c r="C33" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="30">
+      <c r="D33" s="31">
         <v>44592</v>
       </c>
     </row>
@@ -1578,10 +1623,16 @@
       <c r="C34" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="30"/>
+      <c r="D34" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D13:D14"/>
@@ -1590,12 +1641,6 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1607,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD25E0C-56B4-49C9-81FC-B33B23DE8FF6}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -1641,7 +1686,7 @@
       <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="34">
         <v>44593</v>
       </c>
     </row>
@@ -1655,7 +1700,7 @@
       <c r="C3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1667,7 +1712,7 @@
       <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="34">
         <v>44594</v>
       </c>
     </row>
@@ -1681,7 +1726,7 @@
       <c r="C5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1693,7 +1738,7 @@
       <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="34">
         <v>44595</v>
       </c>
     </row>
@@ -1707,7 +1752,7 @@
       <c r="C7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="36"/>
+      <c r="D7" s="34"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1719,7 +1764,7 @@
       <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="34">
         <v>44596</v>
       </c>
     </row>
@@ -1733,7 +1778,7 @@
       <c r="C9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1745,7 +1790,7 @@
       <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="34">
         <v>44599</v>
       </c>
     </row>
@@ -1759,7 +1804,7 @@
       <c r="C11" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="34"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1771,7 +1816,7 @@
       <c r="C12" s="4">
         <v>4</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="34">
         <v>44600</v>
       </c>
     </row>
@@ -1785,7 +1830,7 @@
       <c r="C13" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="36"/>
+      <c r="D13" s="34"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1797,7 +1842,7 @@
       <c r="C14" s="4">
         <v>4</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="34">
         <v>44601</v>
       </c>
     </row>
@@ -1811,7 +1856,7 @@
       <c r="C15" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="34"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -1823,7 +1868,7 @@
       <c r="C16" s="4">
         <v>4</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="34">
         <v>44602</v>
       </c>
     </row>
@@ -1837,7 +1882,7 @@
       <c r="C17" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="36"/>
+      <c r="D17" s="34"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -1849,7 +1894,7 @@
       <c r="C18" s="4">
         <v>4</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="34">
         <v>44603</v>
       </c>
     </row>
@@ -1863,7 +1908,7 @@
       <c r="C19" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="34"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -1875,7 +1920,7 @@
       <c r="C20" s="4">
         <v>4</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="34">
         <v>44606</v>
       </c>
     </row>
@@ -1889,7 +1934,7 @@
       <c r="C21" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="36"/>
+      <c r="D21" s="34"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -1901,7 +1946,7 @@
       <c r="C22" s="4">
         <v>4</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="34">
         <v>44607</v>
       </c>
     </row>
@@ -1915,17 +1960,17 @@
       <c r="C23" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="36"/>
+      <c r="D23" s="34"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="33">
+      <c r="B24" s="35">
         <v>8</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="36">
+      <c r="C24" s="36"/>
+      <c r="D24" s="34">
         <v>44608</v>
       </c>
     </row>
@@ -1933,11 +1978,11 @@
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="34"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -1949,7 +1994,7 @@
       <c r="C26" s="4">
         <v>4</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="34">
         <v>44609</v>
       </c>
     </row>
@@ -1963,7 +2008,7 @@
       <c r="C27" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="36"/>
+      <c r="D27" s="34"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -1975,7 +2020,7 @@
       <c r="C28" s="4">
         <v>4</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="34">
         <v>44610</v>
       </c>
     </row>
@@ -1989,7 +2034,7 @@
       <c r="C29" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="36"/>
+      <c r="D29" s="34"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
@@ -2001,7 +2046,7 @@
       <c r="C30" s="4">
         <v>4</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D30" s="34">
         <v>44613</v>
       </c>
     </row>
@@ -2015,7 +2060,7 @@
       <c r="C31" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="36"/>
+      <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
@@ -2039,7 +2084,7 @@
       <c r="C33" s="4">
         <v>0</v>
       </c>
-      <c r="D33" s="36">
+      <c r="D33" s="34">
         <v>44614</v>
       </c>
     </row>
@@ -2051,7 +2096,7 @@
         <v>63</v>
       </c>
       <c r="C34" s="17"/>
-      <c r="D34" s="36"/>
+      <c r="D34" s="34"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
@@ -2063,7 +2108,7 @@
       <c r="C35" s="4">
         <v>0</v>
       </c>
-      <c r="D35" s="36">
+      <c r="D35" s="34">
         <v>44615</v>
       </c>
     </row>
@@ -2075,7 +2120,7 @@
         <v>64</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="36"/>
+      <c r="D36" s="34"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
@@ -2087,7 +2132,7 @@
       <c r="C37" s="4">
         <v>0</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D37" s="34">
         <v>44616</v>
       </c>
     </row>
@@ -2099,7 +2144,7 @@
         <v>66</v>
       </c>
       <c r="C38" s="17"/>
-      <c r="D38" s="36"/>
+      <c r="D38" s="34"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
@@ -2111,7 +2156,7 @@
       <c r="C39" s="4">
         <v>0</v>
       </c>
-      <c r="D39" s="36">
+      <c r="D39" s="34">
         <v>44617</v>
       </c>
     </row>
@@ -2123,7 +2168,7 @@
         <v>67</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="36"/>
+      <c r="D40" s="34"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
@@ -2135,7 +2180,7 @@
       <c r="C41" s="4">
         <v>0</v>
       </c>
-      <c r="D41" s="36">
+      <c r="D41" s="34">
         <v>44618</v>
       </c>
     </row>
@@ -2147,7 +2192,7 @@
         <v>67</v>
       </c>
       <c r="C42" s="17"/>
-      <c r="D42" s="36"/>
+      <c r="D42" s="34"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
@@ -2159,7 +2204,7 @@
       <c r="C43" s="4">
         <v>0</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D43" s="34">
         <v>44619</v>
       </c>
     </row>
@@ -2171,7 +2216,7 @@
         <v>68</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="36"/>
+      <c r="D44" s="34"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
@@ -2183,7 +2228,7 @@
       <c r="C45" s="4">
         <v>0</v>
       </c>
-      <c r="D45" s="36">
+      <c r="D45" s="34">
         <v>44620</v>
       </c>
     </row>
@@ -2195,10 +2240,22 @@
         <v>69</v>
       </c>
       <c r="C46" s="17"/>
-      <c r="D46" s="36"/>
+      <c r="D46" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="D39:D40"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D43:D44"/>
@@ -2211,18 +2268,6 @@
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2231,10 +2276,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38664062-6459-4C38-9B3B-3A164047A9A0}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2261,11 +2306,11 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="38">
         <v>8</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="36">
+      <c r="C2" s="39"/>
+      <c r="D2" s="34">
         <v>44621</v>
       </c>
     </row>
@@ -2273,11 +2318,11 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -2289,7 +2334,7 @@
       <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="34">
         <v>44622</v>
       </c>
     </row>
@@ -2301,7 +2346,7 @@
         <v>70</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="36"/>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -2313,7 +2358,7 @@
       <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="34">
         <v>44623</v>
       </c>
     </row>
@@ -2325,7 +2370,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="36"/>
+      <c r="D7" s="34"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -2337,7 +2382,7 @@
       <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="34">
         <v>44624</v>
       </c>
     </row>
@@ -2349,7 +2394,7 @@
         <v>72</v>
       </c>
       <c r="C9" s="17"/>
-      <c r="D9" s="36"/>
+      <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -2361,7 +2406,7 @@
       <c r="C10" s="4">
         <v>0</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="34">
         <v>44627</v>
       </c>
     </row>
@@ -2373,7 +2418,7 @@
         <v>76</v>
       </c>
       <c r="C11" s="17"/>
-      <c r="D11" s="36"/>
+      <c r="D11" s="34"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -2385,7 +2430,7 @@
       <c r="C12" s="4">
         <v>0</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="34">
         <v>44628</v>
       </c>
     </row>
@@ -2397,7 +2442,7 @@
         <v>79</v>
       </c>
       <c r="C13" s="17"/>
-      <c r="D13" s="36"/>
+      <c r="D13" s="34"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -2409,7 +2454,7 @@
       <c r="C14" s="4">
         <v>0</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="34">
         <v>44629</v>
       </c>
     </row>
@@ -2421,7 +2466,7 @@
         <v>78</v>
       </c>
       <c r="C15" s="17"/>
-      <c r="D15" s="36"/>
+      <c r="D15" s="34"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -2433,7 +2478,7 @@
       <c r="C16" s="4">
         <v>0</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="34">
         <v>44630</v>
       </c>
     </row>
@@ -2445,7 +2490,7 @@
         <v>77</v>
       </c>
       <c r="C17" s="17"/>
-      <c r="D17" s="36"/>
+      <c r="D17" s="34"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -2457,7 +2502,7 @@
       <c r="C18" s="4">
         <v>4</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="34">
         <v>44631</v>
       </c>
     </row>
@@ -2471,7 +2516,7 @@
       <c r="C19" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="34"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -2483,7 +2528,7 @@
       <c r="C20" s="4">
         <v>0</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="34">
         <v>44634</v>
       </c>
     </row>
@@ -2495,7 +2540,7 @@
         <v>75</v>
       </c>
       <c r="C21" s="17"/>
-      <c r="D21" s="36"/>
+      <c r="D21" s="34"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -2507,7 +2552,7 @@
       <c r="C22" s="4">
         <v>0</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="34">
         <v>44635</v>
       </c>
     </row>
@@ -2519,7 +2564,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="17"/>
-      <c r="D23" s="36"/>
+      <c r="D23" s="34"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -2531,7 +2576,7 @@
       <c r="C24" s="4">
         <v>0</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="34">
         <v>44636</v>
       </c>
     </row>
@@ -2543,7 +2588,7 @@
         <v>82</v>
       </c>
       <c r="C25" s="17"/>
-      <c r="D25" s="36"/>
+      <c r="D25" s="34"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -2555,7 +2600,7 @@
       <c r="C26" s="4">
         <v>0</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="34">
         <v>44637</v>
       </c>
     </row>
@@ -2567,17 +2612,17 @@
         <v>83</v>
       </c>
       <c r="C27" s="17"/>
-      <c r="D27" s="36"/>
+      <c r="D27" s="34"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="33">
+      <c r="B28" s="35">
         <v>8</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="36">
+      <c r="C28" s="36"/>
+      <c r="D28" s="34">
         <v>44638</v>
       </c>
     </row>
@@ -2585,162 +2630,274 @@
       <c r="A29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="36"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="15">
-        <v>2</v>
-      </c>
-      <c r="C30" s="4">
+      <c r="C29" s="36"/>
+      <c r="D29" s="34"/>
+    </row>
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="15">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4">
         <v>6</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D31" s="34">
         <v>44641</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="17" t="s">
+    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C32" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="36"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="15">
-        <v>2</v>
-      </c>
-      <c r="C32" s="4">
+      <c r="D32" s="34"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="15">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4">
         <v>6</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D33" s="34">
         <v>44642</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="17" t="s">
+    <row r="34" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C34" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="36"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="15">
-        <v>2</v>
-      </c>
-      <c r="C34" s="4">
+      <c r="D34" s="34"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="15">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4">
         <v>6</v>
       </c>
-      <c r="D34" s="36">
+      <c r="D35" s="34">
         <v>44643</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="17" t="s">
+    <row r="36" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C36" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="36"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="15">
-        <v>2</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="15">
+        <v>2</v>
+      </c>
+      <c r="C37" s="4">
         <v>6</v>
       </c>
-      <c r="D36" s="36">
+      <c r="D37" s="34">
         <v>44644</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="17" t="s">
+    <row r="38" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C38" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="36"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="33">
-        <v>8</v>
-      </c>
-      <c r="C38" s="34"/>
-      <c r="D38" s="36">
-        <v>44645</v>
-      </c>
+      <c r="D38" s="34"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="36"/>
+        <v>1</v>
+      </c>
+      <c r="B39" s="35">
+        <v>8</v>
+      </c>
+      <c r="C39" s="36"/>
+      <c r="D39" s="34">
+        <v>44645</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="33">
-        <v>8</v>
-      </c>
-      <c r="C40" s="34"/>
-      <c r="D40" s="36">
-        <v>44648</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="36"/>
+      <c r="D40" s="34"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="35">
+        <v>8</v>
+      </c>
+      <c r="C41" s="36"/>
+      <c r="D41" s="34">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="34"/>
-      <c r="D41" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="34"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="15">
+        <v>4</v>
+      </c>
+      <c r="C43" s="4">
+        <v>4</v>
+      </c>
+      <c r="D43" s="34">
+        <v>44649</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="34"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="35">
+        <v>8</v>
+      </c>
+      <c r="C45" s="36"/>
+      <c r="D45" s="34">
+        <v>44650</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="36"/>
+      <c r="D46" s="34"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="15">
+        <v>4</v>
+      </c>
+      <c r="C47" s="4">
+        <v>4</v>
+      </c>
+      <c r="D47" s="34">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="33">
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B2:C2"/>
@@ -2748,30 +2905,98 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B39:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04172E7-821F-44C0-86A6-E4CB79968D23}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>4</v>
+      </c>
+      <c r="D2" s="34">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="34"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="34">
+        <v>44655</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2782,15 +3007,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010071FEBA6E59F1114FA1DBADB5A19192F5" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="68d738ba6abfae8d013aeb1fb6af46ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="33e4e33d-ffb4-4a17-9b1b-478bea8d3710" xmlns:ns4="9120eac6-4b18-4abe-a762-bd257214a810" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dae310c37f0a31cfa956236035f6b2a5" ns3:_="" ns4:_="">
     <xsd:import namespace="33e4e33d-ffb4-4a17-9b1b-478bea8d3710"/>
@@ -2999,6 +3215,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD282290-682D-4720-AA66-05DB34A587D9}">
   <ds:schemaRefs>
@@ -3017,14 +3242,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81EA1DDF-0A41-4AEA-8848-5B89771E278B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{248AF9C3-A2BF-4479-B7A8-B2BDE179A582}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3041,4 +3258,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81EA1DDF-0A41-4AEA-8848-5B89771E278B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>